<commit_message>
Finished Briefing Note Automation
</commit_message>
<xml_diff>
--- a/Briefing Note Enrolment Comparison Table From Previous Academic Year.xlsx
+++ b/Briefing Note Enrolment Comparison Table From Previous Academic Year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://keyanomailca-my.sharepoint.com/personal/bill_guo_keyano_ca/Documents/Documents/KPI-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{125920BB-BE59-4A23-8F35-B4780568970F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EF37E5B-97FA-477B-9271-F6BC689A0BE2}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{125920BB-BE59-4A23-8F35-B4780568970F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83FFD1DD-3CD6-48FC-A294-968E33D7D877}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C89FB34-6A01-4E4F-A7F7-02F8C0983CC0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Category</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>***Please also do not change the name of this sheet.***</t>
+  </si>
+  <si>
+    <t>***No need to fill in grey cells***</t>
   </si>
 </sst>
 </file>
@@ -182,7 +185,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,7 +206,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,107 +379,107 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,7 +817,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,255 +838,258 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="33" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="22" t="s">
+      <c r="D3" s="36"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="24" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="26"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="27"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="39">
         <v>1551</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="39">
         <v>818.56500000000005</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="39">
         <v>987</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="39">
         <v>559.17499999999995</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="39">
         <v>564</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="39">
         <v>259.39</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="39">
         <v>37</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="39">
         <v>11.707000000000001</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="39">
         <v>206</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="39">
         <v>55.935000000000002</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="39">
         <v>425</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="39">
         <v>143.96</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="39">
         <v>960</v>
       </c>
-      <c r="D12" s="37">
+      <c r="D12" s="39">
         <v>547.995</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="37">
+      <c r="C13" s="39">
         <v>175</v>
       </c>
-      <c r="D13" s="37">
+      <c r="D13" s="39">
         <v>126.61</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="37">
+      <c r="C14" s="39">
         <v>1160</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="39">
         <v>502.63299999999998</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="37">
+      <c r="C15" s="39">
         <v>333</v>
       </c>
-      <c r="D15" s="37">
+      <c r="D15" s="39">
         <v>133.40700000000001</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="38"/>
+      <c r="A19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>